<commit_message>
22/04/2021 - Finalizando reportes
</commit_message>
<xml_diff>
--- a/reports/trazabilidad/trazabilidad.xlsx
+++ b/reports/trazabilidad/trazabilidad.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Fecha</t>
   </si>
@@ -37,12 +37,27 @@
     <t>Stock actual</t>
   </si>
   <si>
+    <t>21/04/2021</t>
+  </si>
+  <si>
+    <t>Egreso</t>
+  </si>
+  <si>
+    <t>00000001</t>
+  </si>
+  <si>
+    <t>ASTRI EDITH ANDRADA</t>
+  </si>
+  <si>
+    <t>ZAPATOS</t>
+  </si>
+  <si>
+    <t>UNIDAD</t>
+  </si>
+  <si>
     <t>18/04/2021</t>
   </si>
   <si>
-    <t>Egreso</t>
-  </si>
-  <si>
     <t>00000000</t>
   </si>
   <si>
@@ -52,7 +67,7 @@
     <t>LADRILLOS</t>
   </si>
   <si>
-    <t>"607c802e8fd69700fc909876"</t>
+    <t>BOLSAS</t>
   </si>
   <si>
     <t>Ingreso</t>
@@ -442,7 +457,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="18" customWidth="1"/>
@@ -500,15 +515,15 @@
         <v>200</v>
       </c>
       <c r="H2">
-        <v>100</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
@@ -517,15 +532,41 @@
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G3">
+        <v>200</v>
+      </c>
+      <c r="H3">
         <v>100</v>
       </c>
-      <c r="H3">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+      <c r="H4">
         <v>200</v>
       </c>
     </row>

</xml_diff>

<commit_message>
28/04/2021 - Version 1.1.0
</commit_message>
<xml_diff>
--- a/reports/trazabilidad/trazabilidad.xlsx
+++ b/reports/trazabilidad/trazabilidad.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Fecha</t>
   </si>
@@ -53,30 +53,6 @@
   </si>
   <si>
     <t>UNIDAD</t>
-  </si>
-  <si>
-    <t>18/04/2021</t>
-  </si>
-  <si>
-    <t>00000000</t>
-  </si>
-  <si>
-    <t>MORENO LUCAS OMAR</t>
-  </si>
-  <si>
-    <t>LADRILLOS</t>
-  </si>
-  <si>
-    <t>BOLSAS</t>
-  </si>
-  <si>
-    <t>Ingreso</t>
-  </si>
-  <si>
-    <t>00001-00000611</t>
-  </si>
-  <si>
-    <t>EQUINOCCIO TECHNOLOGY</t>
   </si>
 </sst>
 </file>
@@ -457,7 +433,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="18" customWidth="1"/>
@@ -518,58 +494,6 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3">
-        <v>200</v>
-      </c>
-      <c r="H3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4">
-        <v>100</v>
-      </c>
-      <c r="H4">
-        <v>200</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
10/05/2021 - Para Edificar
</commit_message>
<xml_diff>
--- a/reports/trazabilidad/trazabilidad.xlsx
+++ b/reports/trazabilidad/trazabilidad.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="23">
   <si>
     <t>Fecha</t>
   </si>
@@ -37,22 +37,49 @@
     <t>Stock actual</t>
   </si>
   <si>
-    <t>21/04/2021</t>
+    <t>10/05/2021</t>
   </si>
   <si>
     <t>Egreso</t>
   </si>
   <si>
-    <t>00000001</t>
-  </si>
-  <si>
-    <t>ASTRI EDITH ANDRADA</t>
-  </si>
-  <si>
-    <t>ZAPATOS</t>
-  </si>
-  <si>
-    <t>UNIDAD</t>
+    <t>00000004</t>
+  </si>
+  <si>
+    <t>YAMIL FET</t>
+  </si>
+  <si>
+    <t>CEMENTO HOLCIM BOLSA X 50 KG.</t>
+  </si>
+  <si>
+    <t>UNIDADES</t>
+  </si>
+  <si>
+    <t>BLOCK 19X19X39</t>
+  </si>
+  <si>
+    <t>00000003</t>
+  </si>
+  <si>
+    <t>ARAUJO GUILLERMO</t>
+  </si>
+  <si>
+    <t>Ingreso</t>
+  </si>
+  <si>
+    <t>00002-00000610</t>
+  </si>
+  <si>
+    <t>EQUINOCCIO TECHNOLOGY</t>
+  </si>
+  <si>
+    <t>00000002</t>
+  </si>
+  <si>
+    <t>CALDERON RODRIGO</t>
+  </si>
+  <si>
+    <t>00002-00000615</t>
   </si>
 </sst>
 </file>
@@ -433,7 +460,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H23"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="18" customWidth="1"/>
@@ -488,10 +515,556 @@
         <v>13</v>
       </c>
       <c r="G2">
-        <v>200</v>
+        <v>750</v>
       </c>
       <c r="H2">
-        <v>180</v>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3">
+        <v>1150</v>
+      </c>
+      <c r="H3">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4">
+        <v>1400</v>
+      </c>
+      <c r="H4">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5">
+        <v>850</v>
+      </c>
+      <c r="H5">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6">
+        <v>1500</v>
+      </c>
+      <c r="H6">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7">
+        <v>1000</v>
+      </c>
+      <c r="H7">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8">
+        <v>1780</v>
+      </c>
+      <c r="H8">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <v>1685</v>
+      </c>
+      <c r="H9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10">
+        <v>2000</v>
+      </c>
+      <c r="H10">
+        <v>1685</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11">
+        <v>2000</v>
+      </c>
+      <c r="H11">
+        <v>1780</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12">
+        <v>1500</v>
+      </c>
+      <c r="H12">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <v>1200</v>
+      </c>
+      <c r="H13">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14">
+        <v>1540</v>
+      </c>
+      <c r="H14">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15">
+        <v>1880</v>
+      </c>
+      <c r="H15">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16">
+        <v>2000</v>
+      </c>
+      <c r="H16">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17">
+        <v>2000</v>
+      </c>
+      <c r="H17">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18">
+        <v>2650</v>
+      </c>
+      <c r="H18">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19">
+        <v>2150</v>
+      </c>
+      <c r="H19">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20">
+        <v>2400</v>
+      </c>
+      <c r="H20">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21">
+        <v>2800</v>
+      </c>
+      <c r="H21">
+        <v>2650</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22">
+        <v>800</v>
+      </c>
+      <c r="H22">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23">
+        <v>1700</v>
+      </c>
+      <c r="H23">
+        <v>2400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
11/05/2021 - Para testing
</commit_message>
<xml_diff>
--- a/reports/trazabilidad/trazabilidad.xlsx
+++ b/reports/trazabilidad/trazabilidad.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="28">
   <si>
     <t>Fecha</t>
   </si>
@@ -37,10 +37,31 @@
     <t>Stock actual</t>
   </si>
   <si>
+    <t>11/05/2021</t>
+  </si>
+  <si>
+    <t>Egreso</t>
+  </si>
+  <si>
+    <t>00000006</t>
+  </si>
+  <si>
+    <t>TESTING</t>
+  </si>
+  <si>
+    <t>BLOCK 19X19X39</t>
+  </si>
+  <si>
+    <t>UNIDADES</t>
+  </si>
+  <si>
     <t>10/05/2021</t>
   </si>
   <si>
-    <t>Egreso</t>
+    <t>00000005</t>
+  </si>
+  <si>
+    <t>MORENO YAMILEM</t>
   </si>
   <si>
     <t>00000004</t>
@@ -50,12 +71,6 @@
   </si>
   <si>
     <t>CEMENTO HOLCIM BOLSA X 50 KG.</t>
-  </si>
-  <si>
-    <t>UNIDADES</t>
-  </si>
-  <si>
-    <t>BLOCK 19X19X39</t>
   </si>
   <si>
     <t>00000003</t>
@@ -460,7 +475,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H26"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="18" customWidth="1"/>
@@ -515,10 +530,10 @@
         <v>13</v>
       </c>
       <c r="G2">
-        <v>750</v>
+        <v>900</v>
       </c>
       <c r="H2">
-        <v>700</v>
+        <v>500</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -535,108 +550,108 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
       </c>
       <c r="G3">
-        <v>1150</v>
+        <v>1000</v>
       </c>
       <c r="H3">
-        <v>1100</v>
+        <v>900</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
       </c>
       <c r="G4">
-        <v>1400</v>
+        <v>1100</v>
       </c>
       <c r="H4">
-        <v>1150</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
       </c>
       <c r="G5">
-        <v>850</v>
+        <v>750</v>
       </c>
       <c r="H5">
-        <v>750</v>
+        <v>700</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
       </c>
       <c r="G6">
-        <v>1500</v>
+        <v>1150</v>
       </c>
       <c r="H6">
-        <v>1400</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -645,50 +660,50 @@
         <v>13</v>
       </c>
       <c r="G7">
-        <v>1000</v>
+        <v>1400</v>
       </c>
       <c r="H7">
-        <v>850</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
       </c>
       <c r="G8">
-        <v>1780</v>
+        <v>850</v>
       </c>
       <c r="H8">
-        <v>1500</v>
+        <v>750</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
@@ -697,119 +712,119 @@
         <v>13</v>
       </c>
       <c r="G9">
-        <v>1685</v>
+        <v>1500</v>
       </c>
       <c r="H9">
-        <v>1000</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F10" t="s">
         <v>13</v>
       </c>
       <c r="G10">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="H10">
-        <v>1685</v>
+        <v>850</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F11" t="s">
         <v>13</v>
       </c>
       <c r="G11">
-        <v>2000</v>
+        <v>1780</v>
       </c>
       <c r="H11">
-        <v>1780</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
         <v>19</v>
       </c>
-      <c r="E12" t="s">
-        <v>14</v>
-      </c>
       <c r="F12" t="s">
         <v>13</v>
       </c>
       <c r="G12">
-        <v>1500</v>
+        <v>1685</v>
       </c>
       <c r="H12">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
         <v>19</v>
       </c>
-      <c r="E13" t="s">
-        <v>12</v>
-      </c>
       <c r="F13" t="s">
         <v>13</v>
       </c>
       <c r="G13">
-        <v>1200</v>
+        <v>2000</v>
       </c>
       <c r="H13">
-        <v>2000</v>
+        <v>1685</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -827,128 +842,128 @@
         <v>13</v>
       </c>
       <c r="G14">
-        <v>1540</v>
+        <v>2000</v>
       </c>
       <c r="H14">
-        <v>1200</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F15" t="s">
         <v>13</v>
       </c>
       <c r="G15">
-        <v>1880</v>
+        <v>1500</v>
       </c>
       <c r="H15">
-        <v>1500</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F16" t="s">
         <v>13</v>
       </c>
       <c r="G16">
+        <v>1200</v>
+      </c>
+      <c r="H16">
         <v>2000</v>
-      </c>
-      <c r="H16">
-        <v>1880</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F17" t="s">
         <v>13</v>
       </c>
       <c r="G17">
-        <v>2000</v>
+        <v>1540</v>
       </c>
       <c r="H17">
-        <v>1540</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F18" t="s">
         <v>13</v>
       </c>
       <c r="G18">
-        <v>2650</v>
+        <v>1880</v>
       </c>
       <c r="H18">
-        <v>2000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E19" t="s">
         <v>12</v>
@@ -957,113 +972,191 @@
         <v>13</v>
       </c>
       <c r="G19">
-        <v>2150</v>
+        <v>2000</v>
       </c>
       <c r="H19">
-        <v>2000</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F20" t="s">
         <v>13</v>
       </c>
       <c r="G20">
-        <v>2400</v>
+        <v>2000</v>
       </c>
       <c r="H20">
-        <v>2150</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D21" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F21" t="s">
         <v>13</v>
       </c>
       <c r="G21">
-        <v>2800</v>
+        <v>2650</v>
       </c>
       <c r="H21">
-        <v>2650</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" t="s">
         <v>19</v>
       </c>
-      <c r="E22" t="s">
-        <v>14</v>
-      </c>
       <c r="F22" t="s">
         <v>13</v>
       </c>
       <c r="G22">
-        <v>800</v>
+        <v>2150</v>
       </c>
       <c r="H22">
-        <v>2800</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23">
+        <v>2400</v>
+      </c>
+      <c r="H23">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24">
+        <v>2800</v>
+      </c>
+      <c r="H24">
+        <v>2650</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" t="s">
         <v>22</v>
       </c>
-      <c r="D23" t="s">
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25">
+        <v>800</v>
+      </c>
+      <c r="H25">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" t="s">
         <v>19</v>
       </c>
-      <c r="E23" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23">
+      <c r="F26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26">
         <v>1700</v>
       </c>
-      <c r="H23">
+      <c r="H26">
         <v>2400</v>
       </c>
     </row>

</xml_diff>